<commit_message>
commit alterando o projeto
</commit_message>
<xml_diff>
--- a/PROJETO DE TESTES/[Projeto AeroFree] Projeto de Testes.xlsx
+++ b/PROJETO DE TESTES/[Projeto AeroFree] Projeto de Testes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="EstaPasta_de_trabalho" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" tabRatio="601" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" tabRatio="601" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="5" r:id="rId1"/>
@@ -334,9 +334,6 @@
     <t>marcar feminino, desmarcar e depois marcar masculino</t>
   </si>
   <si>
-    <t>a opção gestante deverar sumir do form após desmarcar feminnino</t>
-  </si>
-  <si>
     <t>desmarcar feminino e marcar masculino</t>
   </si>
   <si>
@@ -473,6 +470,9 @@
   </si>
   <si>
     <t>Exibição da tela no sistema</t>
+  </si>
+  <si>
+    <t>a opção gestante deverar sumir do formato após desmarcar feminino</t>
   </si>
 </sst>
 </file>
@@ -1217,6 +1217,36 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1235,6 +1265,51 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1253,84 +1328,42 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
@@ -1352,12 +1385,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
     </xf>
@@ -1399,399 +1426,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="257">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="10"/>
-      </font>
-    </dxf>
+  <dxfs count="217">
     <dxf>
       <font>
         <b/>
@@ -4572,7 +4212,7 @@
   <sheetPr codeName="Plan3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:IH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
@@ -4605,29 +4245,29 @@
       <c r="A1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="118" t="s">
+      <c r="B1" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="119"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="116" t="s">
+      <c r="C1" s="117"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="104"/>
-      <c r="H1" s="104"/>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="108"/>
-      <c r="M1" s="128" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="130"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="128"/>
       <c r="Q1" s="36"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -4859,23 +4499,23 @@
       <c r="A2" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="121" t="s">
+      <c r="B2" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="122"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-      <c r="I2" s="101"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="133"/>
+      <c r="M2" s="130"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
       <c r="Q2" s="36"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -5104,26 +4744,26 @@
       <c r="IH2" s="1"/>
     </row>
     <row r="3" spans="1:242" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="102"/>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="102"/>
-      <c r="J3" s="102"/>
-      <c r="K3" s="102"/>
-      <c r="L3" s="108"/>
-      <c r="M3" s="106"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
       <c r="Q3" s="36"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -5352,22 +4992,22 @@
       <c r="IH3" s="1"/>
     </row>
     <row r="4" spans="1:242" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="115"/>
-      <c r="B4" s="127"/>
-      <c r="C4" s="119"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="103"/>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="103"/>
-      <c r="K4" s="103"/>
-      <c r="L4" s="109"/>
-      <c r="M4" s="107"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
+      <c r="A4" s="107"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="113"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="132"/>
+      <c r="N4" s="110"/>
+      <c r="O4" s="110"/>
+      <c r="P4" s="110"/>
       <c r="Q4" s="36"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -6094,13 +5734,13 @@
       <c r="IH6" s="1"/>
     </row>
     <row r="7" spans="1:242" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="105" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="105" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="58" t="s">
@@ -6130,7 +5770,7 @@
       <c r="L7" s="49"/>
       <c r="M7" s="50"/>
       <c r="N7" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O7" s="50"/>
       <c r="P7" s="50"/>
@@ -6362,9 +6002,9 @@
       <c r="IH7" s="13"/>
     </row>
     <row r="8" spans="1:242" s="9" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="111"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
       <c r="D8" s="77" t="s">
         <v>45</v>
       </c>
@@ -6630,9 +6270,9 @@
       <c r="IH8" s="13"/>
     </row>
     <row r="9" spans="1:242" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
       <c r="F9" s="48"/>
@@ -7118,14 +6758,14 @@
       <c r="IH10"/>
     </row>
     <row r="11" spans="1:242" s="9" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="112" t="s">
-        <v>147</v>
+      <c r="C11" s="105" t="s">
+        <v>146</v>
       </c>
       <c r="D11" s="58" t="s">
         <v>54</v>
@@ -7372,9 +7012,9 @@
       <c r="IH11" s="13"/>
     </row>
     <row r="12" spans="1:242" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="111"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="58" t="s">
         <v>56</v>
       </c>
@@ -7620,9 +7260,9 @@
       <c r="IH12" s="13"/>
     </row>
     <row r="13" spans="1:242" s="9" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="111"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="100"/>
       <c r="D13" s="46" t="s">
         <v>58</v>
       </c>
@@ -8112,13 +7752,13 @@
       <c r="IH14"/>
     </row>
     <row r="15" spans="1:242" s="9" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="131" t="s">
+      <c r="C15" s="104" t="s">
         <v>61</v>
       </c>
       <c r="D15" s="77" t="s">
@@ -8366,9 +8006,9 @@
       <c r="IH15" s="13"/>
     </row>
     <row r="16" spans="1:242" s="9" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="111"/>
-      <c r="B16" s="113"/>
-      <c r="C16" s="113"/>
+      <c r="A16" s="99"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
       <c r="D16" s="77" t="s">
         <v>45</v>
       </c>
@@ -8614,9 +8254,9 @@
       <c r="IH16" s="13"/>
     </row>
     <row r="17" spans="1:242" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="111"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="113"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="100"/>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
       <c r="F17" s="48"/>
@@ -9102,11 +8742,11 @@
       <c r="IH18"/>
     </row>
     <row r="19" spans="1:242" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="113"/>
-      <c r="C19" s="113"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="100"/>
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
       <c r="F19" s="47"/>
@@ -9348,9 +8988,9 @@
       <c r="IH19" s="13"/>
     </row>
     <row r="20" spans="1:242" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="111"/>
-      <c r="B20" s="113"/>
-      <c r="C20" s="113"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="100"/>
       <c r="D20" s="46"/>
       <c r="E20" s="46"/>
       <c r="F20" s="47"/>
@@ -9592,9 +9232,9 @@
       <c r="IH20" s="13"/>
     </row>
     <row r="21" spans="1:242" s="9" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="111"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="100"/>
+      <c r="C21" s="100"/>
       <c r="D21" s="46"/>
       <c r="E21" s="46"/>
       <c r="F21" s="48"/>
@@ -10080,11 +9720,11 @@
       <c r="IH22"/>
     </row>
     <row r="23" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="132"/>
-      <c r="C23" s="132"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="103"/>
       <c r="D23" s="46"/>
       <c r="E23" s="46"/>
       <c r="F23" s="47"/>
@@ -10101,9 +9741,9 @@
       <c r="Q23" s="36"/>
     </row>
     <row r="24" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A24" s="111"/>
-      <c r="B24" s="133"/>
-      <c r="C24" s="133"/>
+      <c r="A24" s="99"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="101"/>
       <c r="D24" s="46"/>
       <c r="E24" s="46"/>
       <c r="F24" s="47"/>
@@ -10120,9 +9760,9 @@
       <c r="Q24" s="36"/>
     </row>
     <row r="25" spans="1:242" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="111"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="102"/>
+      <c r="C25" s="102"/>
       <c r="D25" s="46"/>
       <c r="E25" s="46"/>
       <c r="F25" s="48"/>
@@ -10158,11 +9798,11 @@
       <c r="Q26" s="56"/>
     </row>
     <row r="27" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="47"/>
@@ -10179,9 +9819,9 @@
       <c r="Q27" s="36"/>
     </row>
     <row r="28" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A28" s="111"/>
-      <c r="B28" s="133"/>
-      <c r="C28" s="133"/>
+      <c r="A28" s="99"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="101"/>
       <c r="D28" s="46"/>
       <c r="E28" s="46"/>
       <c r="F28" s="47"/>
@@ -10198,9 +9838,9 @@
       <c r="Q28" s="36"/>
     </row>
     <row r="29" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A29" s="111"/>
-      <c r="B29" s="113"/>
-      <c r="C29" s="113"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="100"/>
       <c r="D29" s="46"/>
       <c r="E29" s="46"/>
       <c r="F29" s="48"/>
@@ -10218,11 +9858,11 @@
     </row>
     <row r="30" spans="1:242" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A31" s="110" t="s">
+      <c r="A31" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="132"/>
-      <c r="C31" s="132"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="46"/>
       <c r="E31" s="46"/>
       <c r="F31" s="47"/>
@@ -10239,9 +9879,9 @@
       <c r="Q31" s="36"/>
     </row>
     <row r="32" spans="1:242" x14ac:dyDescent="0.2">
-      <c r="A32" s="111"/>
-      <c r="B32" s="133"/>
-      <c r="C32" s="133"/>
+      <c r="A32" s="99"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="101"/>
       <c r="D32" s="46"/>
       <c r="E32" s="46"/>
       <c r="F32" s="47"/>
@@ -10258,9 +9898,9 @@
       <c r="Q32" s="36"/>
     </row>
     <row r="33" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
-      <c r="B33" s="134"/>
-      <c r="C33" s="134"/>
+      <c r="A33" s="99"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="102"/>
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
       <c r="F33" s="48"/>
@@ -10296,11 +9936,11 @@
       <c r="Q34" s="56"/>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="132"/>
-      <c r="C35" s="132"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
       <c r="D35" s="46"/>
       <c r="E35" s="46"/>
       <c r="F35" s="47"/>
@@ -10317,9 +9957,9 @@
       <c r="Q35" s="36"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A36" s="111"/>
-      <c r="B36" s="133"/>
-      <c r="C36" s="133"/>
+      <c r="A36" s="99"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="101"/>
       <c r="D36" s="46"/>
       <c r="E36" s="46"/>
       <c r="F36" s="47"/>
@@ -10336,9 +9976,9 @@
       <c r="Q36" s="36"/>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A37" s="111"/>
-      <c r="B37" s="113"/>
-      <c r="C37" s="113"/>
+      <c r="A37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
       <c r="D37" s="46"/>
       <c r="E37" s="46"/>
       <c r="F37" s="48"/>
@@ -10355,11 +9995,11 @@
       <c r="Q37" s="36"/>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A39" s="110" t="s">
+      <c r="A39" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="133"/>
-      <c r="C39" s="133"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="101"/>
       <c r="D39" s="46"/>
       <c r="E39" s="46"/>
       <c r="F39" s="47"/>
@@ -10375,9 +10015,9 @@
       <c r="P39" s="50"/>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A40" s="111"/>
-      <c r="B40" s="133"/>
-      <c r="C40" s="133"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="101"/>
       <c r="D40" s="46"/>
       <c r="E40" s="46"/>
       <c r="F40" s="47"/>
@@ -10393,9 +10033,9 @@
       <c r="P40" s="51"/>
     </row>
     <row r="41" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
-      <c r="B41" s="134"/>
-      <c r="C41" s="134"/>
+      <c r="A41" s="99"/>
+      <c r="B41" s="102"/>
+      <c r="C41" s="102"/>
       <c r="D41" s="46"/>
       <c r="E41" s="46"/>
       <c r="F41" s="48"/>
@@ -10429,11 +10069,11 @@
       <c r="P42" s="55"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A43" s="110" t="s">
+      <c r="A43" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="113"/>
-      <c r="C43" s="113"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="100"/>
       <c r="D43" s="46"/>
       <c r="E43" s="46"/>
       <c r="F43" s="47"/>
@@ -10449,9 +10089,9 @@
       <c r="P43" s="50"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A44" s="111"/>
-      <c r="B44" s="113"/>
-      <c r="C44" s="113"/>
+      <c r="A44" s="99"/>
+      <c r="B44" s="100"/>
+      <c r="C44" s="100"/>
       <c r="D44" s="46"/>
       <c r="E44" s="46"/>
       <c r="F44" s="47"/>
@@ -10467,9 +10107,9 @@
       <c r="P44" s="51"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A45" s="111"/>
-      <c r="B45" s="113"/>
-      <c r="C45" s="113"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="100"/>
+      <c r="C45" s="100"/>
       <c r="D45" s="46"/>
       <c r="E45" s="46"/>
       <c r="F45" s="48"/>
@@ -10485,11 +10125,11 @@
       <c r="P45" s="50"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A47" s="110" t="s">
+      <c r="A47" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B47" s="113"/>
-      <c r="C47" s="113"/>
+      <c r="B47" s="100"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="46"/>
       <c r="E47" s="46"/>
       <c r="F47" s="47"/>
@@ -10505,9 +10145,9 @@
       <c r="P47" s="50"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A48" s="111"/>
-      <c r="B48" s="113"/>
-      <c r="C48" s="113"/>
+      <c r="A48" s="99"/>
+      <c r="B48" s="100"/>
+      <c r="C48" s="100"/>
       <c r="D48" s="46"/>
       <c r="E48" s="46"/>
       <c r="F48" s="47"/>
@@ -10523,9 +10163,9 @@
       <c r="P48" s="51"/>
     </row>
     <row r="49" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="111"/>
-      <c r="B49" s="113"/>
-      <c r="C49" s="113"/>
+      <c r="A49" s="99"/>
+      <c r="B49" s="100"/>
+      <c r="C49" s="100"/>
       <c r="D49" s="46"/>
       <c r="E49" s="46"/>
       <c r="F49" s="48"/>
@@ -10559,11 +10199,11 @@
       <c r="P50" s="55"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A51" s="110" t="s">
+      <c r="A51" s="98" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="113"/>
-      <c r="C51" s="113"/>
+      <c r="B51" s="100"/>
+      <c r="C51" s="100"/>
       <c r="D51" s="46"/>
       <c r="E51" s="46"/>
       <c r="F51" s="47"/>
@@ -10579,9 +10219,9 @@
       <c r="P51" s="50"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A52" s="111"/>
-      <c r="B52" s="113"/>
-      <c r="C52" s="113"/>
+      <c r="A52" s="99"/>
+      <c r="B52" s="100"/>
+      <c r="C52" s="100"/>
       <c r="D52" s="46"/>
       <c r="E52" s="46"/>
       <c r="F52" s="47"/>
@@ -10597,9 +10237,9 @@
       <c r="P52" s="51"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A53" s="111"/>
-      <c r="B53" s="113"/>
-      <c r="C53" s="113"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="100"/>
       <c r="D53" s="46"/>
       <c r="E53" s="46"/>
       <c r="F53" s="48"/>
@@ -10616,36 +10256,14 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="A43:A45"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="P2:P4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="L1:L4"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -10662,21 +10280,43 @@
     <mergeCell ref="B3:D4"/>
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="J2:J4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="P2:P4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="L1:L4"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="A43:A45"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="G6:K6 M6:P6">
     <cfRule type="cellIs" priority="443" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="256" priority="444" stopIfTrue="1">
+    <cfRule type="expression" dxfId="216" priority="444" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10684,7 +10324,7 @@
     <cfRule type="cellIs" priority="245" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="255" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="215" priority="246" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10692,7 +10332,7 @@
     <cfRule type="cellIs" priority="247" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="254" priority="248" stopIfTrue="1">
+    <cfRule type="expression" dxfId="214" priority="248" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10700,7 +10340,7 @@
     <cfRule type="cellIs" priority="249" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="253" priority="250" stopIfTrue="1">
+    <cfRule type="expression" dxfId="213" priority="250" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10708,7 +10348,7 @@
     <cfRule type="cellIs" priority="199" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="252" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="212" priority="200" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10716,7 +10356,7 @@
     <cfRule type="cellIs" priority="205" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="251" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="211" priority="206" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10724,7 +10364,7 @@
     <cfRule type="cellIs" priority="203" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="250" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="204" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10732,7 +10372,7 @@
     <cfRule type="cellIs" priority="195" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="249" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="196" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10740,7 +10380,7 @@
     <cfRule type="cellIs" priority="191" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="248" priority="192" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="192" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10748,7 +10388,7 @@
     <cfRule type="cellIs" priority="197" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="247" priority="198" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="198" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10756,7 +10396,7 @@
     <cfRule type="cellIs" priority="201" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="246" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="202" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10764,7 +10404,7 @@
     <cfRule type="cellIs" priority="189" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="245" priority="190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="205" priority="190" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10772,7 +10412,7 @@
     <cfRule type="cellIs" priority="187" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="244" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="204" priority="188" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10780,7 +10420,7 @@
     <cfRule type="cellIs" priority="185" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="243" priority="186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="186" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10788,7 +10428,7 @@
     <cfRule type="cellIs" priority="183" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="242" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="184" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10796,7 +10436,7 @@
     <cfRule type="cellIs" priority="181" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="241" priority="182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="182" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10804,7 +10444,7 @@
     <cfRule type="cellIs" priority="179" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="240" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="180" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10812,7 +10452,7 @@
     <cfRule type="cellIs" priority="177" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="239" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="178" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10820,7 +10460,7 @@
     <cfRule type="cellIs" priority="175" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="238" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="198" priority="176" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10828,7 +10468,7 @@
     <cfRule type="cellIs" priority="173" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="237" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="197" priority="174" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10836,7 +10476,7 @@
     <cfRule type="cellIs" priority="171" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="236" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="172" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10844,7 +10484,7 @@
     <cfRule type="cellIs" priority="169" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="235" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="170" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10852,7 +10492,7 @@
     <cfRule type="cellIs" priority="167" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="234" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="168" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10860,7 +10500,7 @@
     <cfRule type="cellIs" priority="165" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="233" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="166" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10868,7 +10508,7 @@
     <cfRule type="cellIs" priority="163" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="232" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="164" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10876,7 +10516,7 @@
     <cfRule type="cellIs" priority="161" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="231" priority="162" stopIfTrue="1">
+    <cfRule type="expression" dxfId="191" priority="162" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10884,7 +10524,7 @@
     <cfRule type="cellIs" priority="159" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="230" priority="160" stopIfTrue="1">
+    <cfRule type="expression" dxfId="190" priority="160" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10892,7 +10532,7 @@
     <cfRule type="cellIs" priority="157" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="229" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="158" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10900,7 +10540,7 @@
     <cfRule type="cellIs" priority="155" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="228" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="156" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10908,7 +10548,7 @@
     <cfRule type="cellIs" priority="153" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="154" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10916,7 +10556,7 @@
     <cfRule type="cellIs" priority="151" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="152" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10924,7 +10564,7 @@
     <cfRule type="cellIs" priority="149" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="150" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="150" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10932,7 +10572,7 @@
     <cfRule type="cellIs" priority="147" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="148" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="148" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10940,7 +10580,7 @@
     <cfRule type="cellIs" priority="145" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="146" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10948,7 +10588,7 @@
     <cfRule type="cellIs" priority="143" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="222" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="182" priority="144" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10956,7 +10596,7 @@
     <cfRule type="cellIs" priority="141" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="221" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="181" priority="142" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10964,7 +10604,7 @@
     <cfRule type="cellIs" priority="139" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="220" priority="140" stopIfTrue="1">
+    <cfRule type="expression" dxfId="180" priority="140" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10972,7 +10612,7 @@
     <cfRule type="cellIs" priority="137" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="219" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="179" priority="138" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10980,7 +10620,7 @@
     <cfRule type="cellIs" priority="135" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="218" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="178" priority="136" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10988,7 +10628,7 @@
     <cfRule type="cellIs" priority="133" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="217" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="177" priority="134" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10996,7 +10636,7 @@
     <cfRule type="cellIs" priority="131" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="216" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="176" priority="132" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11004,7 +10644,7 @@
     <cfRule type="cellIs" priority="129" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="215" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="175" priority="130" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11012,7 +10652,7 @@
     <cfRule type="cellIs" priority="127" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="214" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="174" priority="128" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11020,7 +10660,7 @@
     <cfRule type="cellIs" priority="125" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="213" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="173" priority="126" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11028,7 +10668,7 @@
     <cfRule type="cellIs" priority="123" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="212" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="172" priority="124" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11036,7 +10676,7 @@
     <cfRule type="cellIs" priority="121" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="211" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="171" priority="122" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11044,7 +10684,7 @@
     <cfRule type="cellIs" priority="119" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="210" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="170" priority="120" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11052,7 +10692,7 @@
     <cfRule type="cellIs" priority="117" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="209" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="169" priority="118" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11060,7 +10700,7 @@
     <cfRule type="cellIs" priority="115" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="208" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="168" priority="116" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11068,7 +10708,7 @@
     <cfRule type="cellIs" priority="113" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="207" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="167" priority="114" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11076,7 +10716,7 @@
     <cfRule type="cellIs" priority="111" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="166" priority="112" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11084,7 +10724,7 @@
     <cfRule type="cellIs" priority="109" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="165" priority="110" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11092,7 +10732,7 @@
     <cfRule type="cellIs" priority="107" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="164" priority="108" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11100,7 +10740,7 @@
     <cfRule type="cellIs" priority="105" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="106" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11108,7 +10748,7 @@
     <cfRule type="cellIs" priority="103" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="202" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="104" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11116,7 +10756,7 @@
     <cfRule type="cellIs" priority="101" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="201" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="102" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11124,7 +10764,7 @@
     <cfRule type="cellIs" priority="99" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="100" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11132,7 +10772,7 @@
     <cfRule type="cellIs" priority="97" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="98" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11140,7 +10780,7 @@
     <cfRule type="cellIs" priority="95" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="96" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11148,7 +10788,7 @@
     <cfRule type="cellIs" priority="93" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="94" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11156,7 +10796,7 @@
     <cfRule type="cellIs" priority="91" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="92" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11164,7 +10804,7 @@
     <cfRule type="cellIs" priority="89" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="195" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="90" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11172,7 +10812,7 @@
     <cfRule type="cellIs" priority="87" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="194" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="88" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11180,7 +10820,7 @@
     <cfRule type="cellIs" priority="85" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="193" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="86" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11188,7 +10828,7 @@
     <cfRule type="cellIs" priority="83" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="84" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11196,7 +10836,7 @@
     <cfRule type="cellIs" priority="81" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="82" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11204,7 +10844,7 @@
     <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="80" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11212,7 +10852,7 @@
     <cfRule type="cellIs" priority="77" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="78" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11220,7 +10860,7 @@
     <cfRule type="cellIs" priority="75" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="188" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="76" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11228,7 +10868,7 @@
     <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="187" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="74" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11236,7 +10876,7 @@
     <cfRule type="cellIs" priority="71" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="186" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="72" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11244,7 +10884,7 @@
     <cfRule type="cellIs" priority="69" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="70" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11252,7 +10892,7 @@
     <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="68" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11260,7 +10900,7 @@
     <cfRule type="cellIs" priority="65" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="143" priority="66" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11268,7 +10908,7 @@
     <cfRule type="cellIs" priority="63" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="64" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11276,7 +10916,7 @@
     <cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="181" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="62" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11284,7 +10924,7 @@
     <cfRule type="cellIs" priority="59" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="180" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="60" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11292,7 +10932,7 @@
     <cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="179" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="58" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11300,7 +10940,7 @@
     <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="178" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="56" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11308,7 +10948,7 @@
     <cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="177" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="54" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11316,7 +10956,7 @@
     <cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="176" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="52" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11324,7 +10964,7 @@
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="175" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="50" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11332,7 +10972,7 @@
     <cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="174" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="48" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11340,7 +10980,7 @@
     <cfRule type="cellIs" priority="45" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="173" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="46" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11348,7 +10988,7 @@
     <cfRule type="cellIs" priority="41" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="172" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="42" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11356,7 +10996,7 @@
     <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="171" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="44" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11364,7 +11004,7 @@
     <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="170" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="38" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11372,7 +11012,7 @@
     <cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="169" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="40" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11380,7 +11020,7 @@
     <cfRule type="cellIs" priority="33" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="168" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="34" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11388,7 +11028,7 @@
     <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="167" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="32" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11396,7 +11036,7 @@
     <cfRule type="cellIs" priority="35" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="166" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="36" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11404,7 +11044,7 @@
     <cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="30" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11412,7 +11052,7 @@
     <cfRule type="cellIs" priority="23" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="24" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11420,7 +11060,7 @@
     <cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="18" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11428,7 +11068,7 @@
     <cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="22" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11436,7 +11076,7 @@
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="14" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11444,7 +11084,7 @@
     <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="26" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11452,7 +11092,7 @@
     <cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="28" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11460,7 +11100,7 @@
     <cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="10" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11468,7 +11108,7 @@
     <cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="16" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11476,7 +11116,7 @@
     <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="8" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11484,7 +11124,7 @@
     <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="20" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11492,7 +11132,7 @@
     <cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="12" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11500,7 +11140,7 @@
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="153" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="2" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11508,7 +11148,7 @@
     <cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="6" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11516,7 +11156,7 @@
     <cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="4" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11537,8 +11177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11554,91 +11194,91 @@
       <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="142" t="s">
+      <c r="B1" s="153" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="143"/>
-      <c r="D1" s="144"/>
-      <c r="E1" s="145" t="s">
+      <c r="C1" s="145"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="147" t="s">
+      <c r="F1" s="156" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="147"/>
-      <c r="H1" s="147"/>
-      <c r="I1" s="147"/>
-      <c r="J1" s="147"/>
-      <c r="K1" s="147"/>
-      <c r="L1" s="148"/>
-      <c r="M1" s="150" t="s">
+      <c r="G1" s="156"/>
+      <c r="H1" s="156"/>
+      <c r="I1" s="156"/>
+      <c r="J1" s="156"/>
+      <c r="K1" s="156"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="151"/>
-      <c r="O1" s="151"/>
-      <c r="P1" s="152"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="161"/>
     </row>
     <row r="2" spans="1:17" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="153" t="s">
+      <c r="B2" s="162" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="154"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="156"/>
-      <c r="G2" s="156"/>
-      <c r="H2" s="156"/>
-      <c r="I2" s="156"/>
-      <c r="J2" s="156"/>
-      <c r="K2" s="156"/>
-      <c r="L2" s="148"/>
-      <c r="M2" s="136"/>
-      <c r="N2" s="139"/>
-      <c r="O2" s="139"/>
-      <c r="P2" s="139"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="157"/>
+      <c r="M2" s="147"/>
+      <c r="N2" s="150"/>
+      <c r="O2" s="150"/>
+      <c r="P2" s="150"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="141" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="162"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="145"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="137"/>
-      <c r="N3" s="140"/>
-      <c r="O3" s="140"/>
-      <c r="P3" s="140"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="154"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="148"/>
+      <c r="N3" s="151"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="160"/>
-      <c r="B4" s="164"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="158"/>
-      <c r="G4" s="158"/>
-      <c r="H4" s="158"/>
-      <c r="I4" s="158"/>
-      <c r="J4" s="158"/>
-      <c r="K4" s="158"/>
-      <c r="L4" s="149"/>
-      <c r="M4" s="138"/>
-      <c r="N4" s="141"/>
-      <c r="O4" s="141"/>
-      <c r="P4" s="141"/>
+      <c r="A4" s="140"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="145"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
+      <c r="K4" s="167"/>
+      <c r="L4" s="158"/>
+      <c r="M4" s="149"/>
+      <c r="N4" s="152"/>
+      <c r="O4" s="152"/>
+      <c r="P4" s="152"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="62"/>
@@ -11687,13 +11327,13 @@
       <c r="P6" s="70"/>
     </row>
     <row r="7" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="131" t="s">
+      <c r="B7" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="105" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="58" t="s">
@@ -11722,9 +11362,9 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="111"/>
-      <c r="B8" s="113"/>
-      <c r="C8" s="113"/>
+      <c r="A8" s="99"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="100"/>
       <c r="D8" s="77"/>
       <c r="E8" s="46"/>
       <c r="F8" s="80"/>
@@ -11741,9 +11381,9 @@
       <c r="Q8" s="81"/>
     </row>
     <row r="9" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="111"/>
-      <c r="B9" s="113"/>
-      <c r="C9" s="113"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="100"/>
       <c r="D9" s="46"/>
       <c r="E9" s="46"/>
       <c r="F9" s="82"/>
@@ -11779,13 +11419,13 @@
       <c r="Q10" s="86"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="131" t="s">
+      <c r="B11" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="165" t="s">
+      <c r="C11" s="136" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="77" t="s">
@@ -11822,9 +11462,9 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="111"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="166"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="137"/>
       <c r="D12" s="77"/>
       <c r="E12" s="77"/>
       <c r="F12" s="80"/>
@@ -11841,9 +11481,9 @@
       <c r="Q12" s="83"/>
     </row>
     <row r="13" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="111"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="167"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="138"/>
       <c r="D13" s="46"/>
       <c r="E13" s="46"/>
       <c r="F13" s="82"/>
@@ -11879,13 +11519,13 @@
       <c r="Q14" s="86"/>
     </row>
     <row r="15" spans="1:17" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="110" t="s">
+      <c r="A15" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="131" t="s">
+      <c r="B15" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="165" t="s">
+      <c r="C15" s="136" t="s">
         <v>66</v>
       </c>
       <c r="D15" s="77" t="s">
@@ -11912,9 +11552,9 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="110"/>
-      <c r="B16" s="131"/>
-      <c r="C16" s="166"/>
+      <c r="A16" s="98"/>
+      <c r="B16" s="104"/>
+      <c r="C16" s="137"/>
       <c r="D16" s="77" t="s">
         <v>81</v>
       </c>
@@ -11937,9 +11577,9 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="111"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="166"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="100"/>
+      <c r="C17" s="137"/>
       <c r="D17" s="77" t="s">
         <v>83</v>
       </c>
@@ -11964,9 +11604,9 @@
       </c>
     </row>
     <row r="18" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="111"/>
-      <c r="B18" s="113"/>
-      <c r="C18" s="166"/>
+      <c r="A18" s="99"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="137"/>
       <c r="D18" s="77" t="s">
         <v>86</v>
       </c>
@@ -11991,9 +11631,9 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="111"/>
-      <c r="B19" s="113"/>
-      <c r="C19" s="167"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="77" t="s">
         <v>88</v>
       </c>
@@ -12037,13 +11677,13 @@
       <c r="Q20" s="86"/>
     </row>
     <row r="21" spans="1:17" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="110" t="s">
+      <c r="A21" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="131" t="s">
+      <c r="B21" s="104" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="113" t="s">
+      <c r="C21" s="100" t="s">
         <v>66</v>
       </c>
       <c r="D21" s="46" t="s">
@@ -12072,9 +11712,9 @@
       </c>
     </row>
     <row r="22" spans="1:17" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="111"/>
-      <c r="B22" s="113"/>
-      <c r="C22" s="113"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="46"/>
       <c r="E22" s="46"/>
       <c r="F22" s="80"/>
@@ -12091,9 +11731,9 @@
       <c r="Q22" s="83"/>
     </row>
     <row r="23" spans="1:17" ht="13.5" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="111"/>
-      <c r="B23" s="113"/>
-      <c r="C23" s="113"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
       <c r="D23" s="46"/>
       <c r="E23" s="46"/>
       <c r="F23" s="82"/>
@@ -12129,13 +11769,13 @@
       <c r="Q24" s="86"/>
     </row>
     <row r="25" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="110" t="s">
+      <c r="A25" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="132" t="s">
+      <c r="B25" s="103" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="113" t="s">
+      <c r="C25" s="100" t="s">
         <v>66</v>
       </c>
       <c r="D25" s="46" t="s">
@@ -12164,17 +11804,17 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="111"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="113"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="46" t="s">
         <v>101</v>
       </c>
       <c r="E26" s="92" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="80" t="s">
         <v>102</v>
-      </c>
-      <c r="F26" s="80" t="s">
-        <v>103</v>
       </c>
       <c r="G26" s="47"/>
       <c r="H26" s="48"/>
@@ -12183,7 +11823,7 @@
       <c r="K26" s="48"/>
       <c r="L26" s="49"/>
       <c r="M26" s="93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N26" s="94"/>
       <c r="O26" s="94"/>
@@ -12193,17 +11833,17 @@
       </c>
     </row>
     <row r="27" spans="1:17" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="111"/>
-      <c r="B27" s="134"/>
-      <c r="C27" s="113"/>
+      <c r="A27" s="99"/>
+      <c r="B27" s="102"/>
+      <c r="C27" s="100"/>
       <c r="D27" s="77" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="77" t="s">
+      <c r="F27" s="82" t="s">
         <v>106</v>
-      </c>
-      <c r="F27" s="82" t="s">
-        <v>107</v>
       </c>
       <c r="G27" s="48"/>
       <c r="H27" s="48"/>
@@ -12212,7 +11852,7 @@
       <c r="K27" s="48"/>
       <c r="L27" s="49"/>
       <c r="M27" s="50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N27" s="51"/>
       <c r="O27" s="51"/>
@@ -12238,20 +11878,20 @@
       <c r="P28" s="75"/>
     </row>
     <row r="29" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="110" t="s">
+      <c r="A29" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="131" t="s">
+      <c r="B29" s="104" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="105" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="C29" s="112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="77" t="s">
-        <v>138</v>
-      </c>
       <c r="E29" s="77" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="71"/>
       <c r="G29" s="71"/>
@@ -12266,14 +11906,14 @@
       <c r="P29" s="73"/>
     </row>
     <row r="30" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="111"/>
-      <c r="B30" s="113"/>
-      <c r="C30" s="113"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="100"/>
+      <c r="C30" s="100"/>
       <c r="D30" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F30" s="71"/>
       <c r="G30" s="71"/>
@@ -12288,14 +11928,14 @@
       <c r="P30" s="73"/>
     </row>
     <row r="31" spans="1:17" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="111"/>
-      <c r="B31" s="113"/>
-      <c r="C31" s="113"/>
+      <c r="A31" s="99"/>
+      <c r="B31" s="100"/>
+      <c r="C31" s="100"/>
       <c r="D31" s="58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F31" s="71"/>
       <c r="G31" s="71"/>
@@ -12328,20 +11968,20 @@
       <c r="P32" s="75"/>
     </row>
     <row r="33" spans="1:16" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="110" t="s">
+      <c r="A33" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="131" t="s">
-        <v>142</v>
-      </c>
-      <c r="C33" s="112" t="s">
-        <v>139</v>
+      <c r="B33" s="104" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" s="105" t="s">
+        <v>138</v>
       </c>
       <c r="D33" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="77" t="s">
         <v>112</v>
-      </c>
-      <c r="E33" s="77" t="s">
-        <v>113</v>
       </c>
       <c r="F33" s="71"/>
       <c r="G33" s="71"/>
@@ -12356,9 +11996,9 @@
       <c r="P33" s="73"/>
     </row>
     <row r="34" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="111"/>
-      <c r="B34" s="113"/>
-      <c r="C34" s="113"/>
+      <c r="A34" s="99"/>
+      <c r="B34" s="100"/>
+      <c r="C34" s="100"/>
       <c r="D34" s="77"/>
       <c r="E34" s="58"/>
       <c r="F34" s="71"/>
@@ -12374,9 +12014,9 @@
       <c r="P34" s="73"/>
     </row>
     <row r="35" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="113"/>
+      <c r="A35" s="99"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="100"/>
       <c r="D35" s="77"/>
       <c r="E35" s="46"/>
       <c r="F35" s="71"/>
@@ -12410,20 +12050,20 @@
       <c r="P36" s="76"/>
     </row>
     <row r="37" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="110" t="s">
+      <c r="A37" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="104" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="105" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D37" s="77" t="s">
+      <c r="E37" s="77" t="s">
         <v>116</v>
-      </c>
-      <c r="E37" s="77" t="s">
-        <v>117</v>
       </c>
       <c r="F37" s="71"/>
       <c r="G37" s="71"/>
@@ -12438,9 +12078,9 @@
       <c r="P37" s="73"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A38" s="111"/>
-      <c r="B38" s="113"/>
-      <c r="C38" s="113"/>
+      <c r="A38" s="99"/>
+      <c r="B38" s="100"/>
+      <c r="C38" s="100"/>
       <c r="D38" s="77"/>
       <c r="E38" s="77"/>
       <c r="F38" s="71"/>
@@ -12456,9 +12096,9 @@
       <c r="P38" s="73"/>
     </row>
     <row r="39" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="111"/>
-      <c r="B39" s="113"/>
-      <c r="C39" s="113"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="100"/>
+      <c r="C39" s="100"/>
       <c r="D39" s="77"/>
       <c r="E39" s="46"/>
       <c r="F39" s="71"/>
@@ -12492,20 +12132,20 @@
       <c r="P40" s="75"/>
     </row>
     <row r="41" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="110" t="s">
+      <c r="A41" s="98" t="s">
         <v>27</v>
       </c>
       <c r="B41" s="135" t="s">
-        <v>143</v>
-      </c>
-      <c r="C41" s="165" t="s">
-        <v>139</v>
+        <v>142</v>
+      </c>
+      <c r="C41" s="136" t="s">
+        <v>138</v>
       </c>
       <c r="D41" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="58" t="s">
         <v>119</v>
-      </c>
-      <c r="E41" s="58" t="s">
-        <v>120</v>
       </c>
       <c r="F41" s="71"/>
       <c r="G41" s="71"/>
@@ -12520,14 +12160,14 @@
       <c r="P41" s="73"/>
     </row>
     <row r="42" spans="1:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="111"/>
-      <c r="B42" s="133"/>
-      <c r="C42" s="166"/>
+      <c r="A42" s="99"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="137"/>
       <c r="D42" s="58" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="58" t="s">
         <v>121</v>
-      </c>
-      <c r="E42" s="58" t="s">
-        <v>122</v>
       </c>
       <c r="F42" s="71"/>
       <c r="G42" s="71"/>
@@ -12542,9 +12182,9 @@
       <c r="P42" s="73"/>
     </row>
     <row r="43" spans="1:16" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="111"/>
-      <c r="B43" s="134"/>
-      <c r="C43" s="167"/>
+      <c r="A43" s="99"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="138"/>
       <c r="D43" s="46"/>
       <c r="E43" s="46"/>
       <c r="F43" s="71"/>
@@ -12567,20 +12207,20 @@
       <c r="E44" s="54"/>
     </row>
     <row r="45" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="110" t="s">
-        <v>114</v>
+      <c r="A45" s="98" t="s">
+        <v>113</v>
       </c>
       <c r="B45" s="135" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="112" t="s">
-        <v>139</v>
+        <v>143</v>
+      </c>
+      <c r="C45" s="105" t="s">
+        <v>138</v>
       </c>
       <c r="D45" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="58" t="s">
         <v>123</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>124</v>
       </c>
       <c r="F45" s="71"/>
       <c r="G45" s="71"/>
@@ -12595,14 +12235,14 @@
       <c r="P45" s="73"/>
     </row>
     <row r="46" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="111"/>
-      <c r="B46" s="133"/>
-      <c r="C46" s="113"/>
+      <c r="A46" s="99"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="100"/>
       <c r="D46" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="58" t="s">
         <v>125</v>
-      </c>
-      <c r="E46" s="58" t="s">
-        <v>126</v>
       </c>
       <c r="F46" s="71"/>
       <c r="G46" s="71"/>
@@ -12617,14 +12257,14 @@
       <c r="P46" s="73"/>
     </row>
     <row r="47" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="111"/>
-      <c r="B47" s="113"/>
-      <c r="C47" s="113"/>
+      <c r="A47" s="99"/>
+      <c r="B47" s="100"/>
+      <c r="C47" s="100"/>
       <c r="D47" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="E47" s="58" t="s">
         <v>127</v>
-      </c>
-      <c r="E47" s="58" t="s">
-        <v>128</v>
       </c>
       <c r="F47" s="71"/>
       <c r="G47" s="71"/>
@@ -12646,20 +12286,20 @@
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="110" t="s">
-        <v>118</v>
+      <c r="A49" s="98" t="s">
+        <v>117</v>
       </c>
       <c r="B49" s="135" t="s">
-        <v>145</v>
-      </c>
-      <c r="C49" s="112" t="s">
-        <v>139</v>
+        <v>144</v>
+      </c>
+      <c r="C49" s="105" t="s">
+        <v>138</v>
       </c>
       <c r="D49" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="E49" s="58" t="s">
         <v>129</v>
-      </c>
-      <c r="E49" s="58" t="s">
-        <v>130</v>
       </c>
       <c r="F49" s="71"/>
       <c r="G49" s="71"/>
@@ -12674,14 +12314,14 @@
       <c r="P49" s="73"/>
     </row>
     <row r="50" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="111"/>
-      <c r="B50" s="133"/>
-      <c r="C50" s="113"/>
+      <c r="A50" s="99"/>
+      <c r="B50" s="101"/>
+      <c r="C50" s="100"/>
       <c r="D50" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="58" t="s">
         <v>131</v>
-      </c>
-      <c r="E50" s="58" t="s">
-        <v>132</v>
       </c>
       <c r="F50" s="71"/>
       <c r="G50" s="71"/>
@@ -12696,11 +12336,11 @@
       <c r="P50" s="73"/>
     </row>
     <row r="51" spans="1:16" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="111"/>
-      <c r="B51" s="134"/>
-      <c r="C51" s="113"/>
+      <c r="A51" s="99"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="100"/>
       <c r="D51" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E51" s="46"/>
       <c r="F51" s="71"/>
@@ -12723,20 +12363,20 @@
       <c r="E52" s="54"/>
     </row>
     <row r="53" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="110" t="s">
+      <c r="A53" s="98" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="135" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="105" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="77" t="s">
         <v>134</v>
       </c>
-      <c r="B53" s="135" t="s">
-        <v>146</v>
-      </c>
-      <c r="C53" s="112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="77" t="s">
+      <c r="E53" s="77" t="s">
         <v>135</v>
-      </c>
-      <c r="E53" s="77" t="s">
-        <v>136</v>
       </c>
       <c r="F53" s="71"/>
       <c r="G53" s="71"/>
@@ -12751,9 +12391,9 @@
       <c r="P53" s="73"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="111"/>
-      <c r="B54" s="133"/>
-      <c r="C54" s="113"/>
+      <c r="A54" s="99"/>
+      <c r="B54" s="101"/>
+      <c r="C54" s="100"/>
       <c r="D54" s="46"/>
       <c r="E54" s="46"/>
       <c r="F54" s="71"/>
@@ -12769,9 +12409,9 @@
       <c r="P54" s="73"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A55" s="111"/>
-      <c r="B55" s="113"/>
-      <c r="C55" s="113"/>
+      <c r="A55" s="99"/>
+      <c r="B55" s="100"/>
+      <c r="C55" s="100"/>
       <c r="D55" s="46"/>
       <c r="E55" s="46"/>
       <c r="F55" s="71"/>
@@ -12788,35 +12428,15 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D4"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="C49:C51"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="O2:O4"/>
@@ -12833,21 +12453,41 @@
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="J2:J4"/>
     <mergeCell ref="K2:K4"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D4"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="C41:C43"/>
   </mergeCells>
   <conditionalFormatting sqref="G6:K6 M6:P6">
     <cfRule type="cellIs" priority="347" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="348" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="348" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12855,7 +12495,7 @@
     <cfRule type="cellIs" priority="243" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="244" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12863,7 +12503,7 @@
     <cfRule type="cellIs" priority="241" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="242" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12871,7 +12511,7 @@
     <cfRule type="cellIs" priority="239" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="147" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="240" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12879,7 +12519,7 @@
     <cfRule type="cellIs" priority="231" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="232" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="232" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12887,7 +12527,7 @@
     <cfRule type="cellIs" priority="229" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="230" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="230" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12895,7 +12535,7 @@
     <cfRule type="cellIs" priority="225" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="226" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="226" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12903,7 +12543,7 @@
     <cfRule type="cellIs" priority="223" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="224" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="224" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12911,7 +12551,7 @@
     <cfRule type="cellIs" priority="221" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="222" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="222" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12919,7 +12559,7 @@
     <cfRule type="cellIs" priority="219" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="220" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="220" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12927,7 +12567,7 @@
     <cfRule type="cellIs" priority="217" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="140" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="218" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12935,7 +12575,7 @@
     <cfRule type="cellIs" priority="207" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="139" priority="208" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="208" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12943,7 +12583,7 @@
     <cfRule type="cellIs" priority="205" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="206" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12951,7 +12591,7 @@
     <cfRule type="cellIs" priority="203" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="204" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12959,7 +12599,7 @@
     <cfRule type="cellIs" priority="195" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="196" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="196" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12967,7 +12607,7 @@
     <cfRule type="cellIs" priority="193" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="194" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="194" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12975,7 +12615,7 @@
     <cfRule type="cellIs" priority="189" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="190" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="190" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12983,7 +12623,7 @@
     <cfRule type="cellIs" priority="187" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="188" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="188" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12991,7 +12631,7 @@
     <cfRule type="cellIs" priority="185" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="132" priority="186" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="186" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12999,7 +12639,7 @@
     <cfRule type="cellIs" priority="183" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="184" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="184" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13007,7 +12647,7 @@
     <cfRule type="cellIs" priority="181" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="182" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="182" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13015,7 +12655,7 @@
     <cfRule type="cellIs" priority="179" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="180" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13023,7 +12663,7 @@
     <cfRule type="cellIs" priority="177" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="178" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13031,7 +12671,7 @@
     <cfRule type="cellIs" priority="175" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="176" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13039,7 +12679,7 @@
     <cfRule type="cellIs" priority="173" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="174" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13047,7 +12687,7 @@
     <cfRule type="cellIs" priority="171" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="172" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="172" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13055,7 +12695,7 @@
     <cfRule type="cellIs" priority="169" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="170" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="170" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13063,7 +12703,7 @@
     <cfRule type="cellIs" priority="167" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="168" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="168" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13071,7 +12711,7 @@
     <cfRule type="cellIs" priority="165" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="166" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="166" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13079,7 +12719,7 @@
     <cfRule type="cellIs" priority="163" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="164" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="164" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13087,7 +12727,7 @@
     <cfRule type="cellIs" priority="161" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="162" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="162" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13095,7 +12735,7 @@
     <cfRule type="cellIs" priority="159" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="160" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="160" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13103,7 +12743,7 @@
     <cfRule type="cellIs" priority="157" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="158" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="158" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13111,7 +12751,7 @@
     <cfRule type="cellIs" priority="155" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="156" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="156" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13119,7 +12759,7 @@
     <cfRule type="cellIs" priority="153" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="154" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="154" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13127,7 +12767,7 @@
     <cfRule type="cellIs" priority="151" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="152" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13135,7 +12775,7 @@
     <cfRule type="cellIs" priority="149" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="150" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="150" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13143,7 +12783,7 @@
     <cfRule type="cellIs" priority="147" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="148" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="148" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13151,7 +12791,7 @@
     <cfRule type="cellIs" priority="145" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="112" priority="146" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="146" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13159,7 +12799,7 @@
     <cfRule type="cellIs" priority="61" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="62" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="62" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13167,7 +12807,7 @@
     <cfRule type="cellIs" priority="143" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="144" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="144" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13175,7 +12815,7 @@
     <cfRule type="cellIs" priority="139" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="140" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="140" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13183,7 +12823,7 @@
     <cfRule type="cellIs" priority="141" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="142" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13191,7 +12831,7 @@
     <cfRule type="cellIs" priority="135" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="136" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13199,7 +12839,7 @@
     <cfRule type="cellIs" priority="137" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="138" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13207,7 +12847,7 @@
     <cfRule type="cellIs" priority="131" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="132" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="132" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13215,7 +12855,7 @@
     <cfRule type="cellIs" priority="129" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="130" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="130" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13223,7 +12863,7 @@
     <cfRule type="cellIs" priority="133" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="134" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="134" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13231,7 +12871,7 @@
     <cfRule type="cellIs" priority="127" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="128" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="128" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13239,7 +12879,7 @@
     <cfRule type="cellIs" priority="121" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="122" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="122" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13247,7 +12887,7 @@
     <cfRule type="cellIs" priority="123" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="124" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="124" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13255,7 +12895,7 @@
     <cfRule type="cellIs" priority="125" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="126" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="126" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13263,7 +12903,7 @@
     <cfRule type="cellIs" priority="115" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="116" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13271,7 +12911,7 @@
     <cfRule type="cellIs" priority="109" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="110" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13279,7 +12919,7 @@
     <cfRule type="cellIs" priority="113" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="114" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="114" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13287,7 +12927,7 @@
     <cfRule type="cellIs" priority="105" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="106" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="106" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13295,7 +12935,7 @@
     <cfRule type="cellIs" priority="117" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="118" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="118" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13303,7 +12943,7 @@
     <cfRule type="cellIs" priority="119" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="120" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="120" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13311,7 +12951,7 @@
     <cfRule type="cellIs" priority="101" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="102" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13319,7 +12959,7 @@
     <cfRule type="cellIs" priority="107" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="108" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13327,7 +12967,7 @@
     <cfRule type="cellIs" priority="99" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="100" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="100" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13335,7 +12975,7 @@
     <cfRule type="cellIs" priority="111" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="112" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13343,7 +12983,7 @@
     <cfRule type="cellIs" priority="91" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="92" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13351,7 +12991,7 @@
     <cfRule type="cellIs" priority="97" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="98" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13359,7 +12999,7 @@
     <cfRule type="cellIs" priority="103" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="104" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="104" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13367,7 +13007,7 @@
     <cfRule type="cellIs" priority="95" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="96" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13375,7 +13015,7 @@
     <cfRule type="cellIs" priority="87" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="88" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="88" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13383,7 +13023,7 @@
     <cfRule type="cellIs" priority="85" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="86" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="86" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13391,7 +13031,7 @@
     <cfRule type="cellIs" priority="89" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="90" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="90" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13399,7 +13039,7 @@
     <cfRule type="cellIs" priority="93" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="94" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13407,7 +13047,7 @@
     <cfRule type="cellIs" priority="83" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="84" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13415,7 +13055,7 @@
     <cfRule type="cellIs" priority="81" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="82" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13423,7 +13063,7 @@
     <cfRule type="cellIs" priority="79" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="80" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13431,7 +13071,7 @@
     <cfRule type="cellIs" priority="77" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="78" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13439,7 +13079,7 @@
     <cfRule type="cellIs" priority="75" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="76" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="76" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13447,7 +13087,7 @@
     <cfRule type="cellIs" priority="73" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="74" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13455,7 +13095,7 @@
     <cfRule type="cellIs" priority="71" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="72" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13463,7 +13103,7 @@
     <cfRule type="cellIs" priority="69" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="70" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="70" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13471,7 +13111,7 @@
     <cfRule type="cellIs" priority="63" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="64" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13479,7 +13119,7 @@
     <cfRule type="cellIs" priority="67" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="68" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="68" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13487,7 +13127,7 @@
     <cfRule type="cellIs" priority="65" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="66" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13495,7 +13135,7 @@
     <cfRule type="cellIs" priority="59" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="60" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13503,7 +13143,7 @@
     <cfRule type="cellIs" priority="57" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="58" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13511,7 +13151,7 @@
     <cfRule type="cellIs" priority="55" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="56" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13519,7 +13159,7 @@
     <cfRule type="cellIs" priority="53" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="54" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13527,7 +13167,7 @@
     <cfRule type="cellIs" priority="51" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="52" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13535,7 +13175,7 @@
     <cfRule type="cellIs" priority="49" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="50" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13543,7 +13183,7 @@
     <cfRule type="cellIs" priority="47" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="48" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13551,7 +13191,7 @@
     <cfRule type="cellIs" priority="45" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="46" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="46" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13559,7 +13199,7 @@
     <cfRule type="cellIs" priority="43" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="44" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13567,7 +13207,7 @@
     <cfRule type="cellIs" priority="41" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="42" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13575,7 +13215,7 @@
     <cfRule type="cellIs" priority="39" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="40" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13583,7 +13223,7 @@
     <cfRule type="cellIs" priority="37" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="38" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13591,7 +13231,7 @@
     <cfRule type="cellIs" priority="35" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="36" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13599,7 +13239,7 @@
     <cfRule type="cellIs" priority="33" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="34" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13607,7 +13247,7 @@
     <cfRule type="cellIs" priority="31" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="32" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13615,7 +13255,7 @@
     <cfRule type="cellIs" priority="29" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13623,7 +13263,7 @@
     <cfRule type="cellIs" priority="27" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="28" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13631,7 +13271,7 @@
     <cfRule type="cellIs" priority="25" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="26" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13639,7 +13279,7 @@
     <cfRule type="cellIs" priority="23" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="24" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13647,7 +13287,7 @@
     <cfRule type="cellIs" priority="21" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="22" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13655,7 +13295,7 @@
     <cfRule type="cellIs" priority="19" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="20" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13663,7 +13303,7 @@
     <cfRule type="cellIs" priority="17" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="18" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13671,7 +13311,7 @@
     <cfRule type="cellIs" priority="15" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="16" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13679,7 +13319,7 @@
     <cfRule type="cellIs" priority="13" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13687,7 +13327,7 @@
     <cfRule type="cellIs" priority="11" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="12" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13695,7 +13335,7 @@
     <cfRule type="cellIs" priority="9" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="10" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13703,7 +13343,7 @@
     <cfRule type="cellIs" priority="7" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="8" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13711,7 +13351,7 @@
     <cfRule type="cellIs" priority="5" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13719,7 +13359,7 @@
     <cfRule type="cellIs" priority="3" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13727,7 +13367,7 @@
     <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>#REF!="S"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>